<commit_message>
RL_env v9, v10, v11
Integration of uncertainties with Sobol sequence.
Actions: limit gwp, limit coal, lfo and ng
</commit_message>
<xml_diff>
--- a/uncertainties/uc_final.xlsx
+++ b/uncertainties/uc_final.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xrixhon/Development/GitKraken/EnergyScope_pathway/uncertainties/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6039B6D4-1635-7848-BA48-96AE29B94F13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55A2C85E-3FC4-7949-A57A-4AECC480459D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1380" yWindow="500" windowWidth="27420" windowHeight="17500" activeTab="1" xr2:uid="{0538DB9B-7B42-9049-9301-4FBFACF63AD6}"/>
+    <workbookView xWindow="3400" yWindow="-18560" windowWidth="27420" windowHeight="17500" activeTab="1" xr2:uid="{0538DB9B-7B42-9049-9301-4FBFACF63AD6}"/>
   </bookViews>
   <sheets>
     <sheet name="READ_ME" sheetId="11" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="396" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="136">
   <si>
     <t>Parameter</t>
   </si>
@@ -90,108 +90,27 @@
     <t>delta_change_pax</t>
   </si>
   <si>
-    <t>"Investment cost of FC propulsion system"</t>
-  </si>
-  <si>
     <t>c_op_import</t>
   </si>
   <si>
-    <t>"Investment cost of cars"</t>
-  </si>
-  <si>
     <t>c_inv_thermal_plants</t>
   </si>
   <si>
-    <t>"Variability in maintenance cost"</t>
-  </si>
-  <si>
-    <t>"Investment cost to increase efficiency of the system"</t>
-  </si>
-  <si>
     <t>c_inv_DHN</t>
   </si>
   <si>
-    <t>"Interest rate"</t>
-  </si>
-  <si>
-    <t>"Investment cost of IC propulsion system"</t>
-  </si>
-  <si>
-    <t>"Investment cost of e-propulsion system"</t>
-  </si>
-  <si>
-    <t>"Maximum share of pax-transport supplied by public transport"</t>
-  </si>
-  <si>
     <t>NA</t>
   </si>
   <si>
-    <t>"Operational cost of imported electricity"</t>
-  </si>
-  <si>
-    <t>"Efficiency of FC propulsion system"</t>
-  </si>
-  <si>
     <t>eff_FC_CAR</t>
   </si>
   <si>
-    <t>"Efficiency of e-propulsion system"</t>
-  </si>
-  <si>
-    <t>"Investment cost of PV"</t>
-  </si>
-  <si>
-    <t>"End-use demand of passenger mobility"</t>
-  </si>
-  <si>
     <t>EUD_transport</t>
   </si>
   <si>
-    <t>"Investment in the power grid'</t>
-  </si>
-  <si>
-    <t>"End-use demand of space heating"</t>
-  </si>
-  <si>
-    <t>"Investment cost of buses"</t>
-  </si>
-  <si>
-    <t>"Maximum capacity of onshore wind"</t>
-  </si>
-  <si>
-    <t>"Available imported electricity"</t>
-  </si>
-  <si>
     <t>avail_WOOD</t>
   </si>
   <si>
-    <t>"Load factor of PV"</t>
-  </si>
-  <si>
-    <t>"Operation cost of imported biofuels"</t>
-  </si>
-  <si>
-    <t>"Operational cost of imported electrofuels"</t>
-  </si>
-  <si>
-    <t>"Load factor of wind turbines"</t>
-  </si>
-  <si>
-    <t>"Maximum capacity of offshore wind"</t>
-  </si>
-  <si>
-    <t>"Extra investment in the power grid due to VRES"</t>
-  </si>
-  <si>
-    <t>"Change of share of freight transport"</t>
-  </si>
-  <si>
-    <t>"Change of share of passenger transport"</t>
-  </si>
-  <si>
-    <t>"Change of share of low-temperature heat"</t>
-  </si>
-  <si>
     <t>c_op_hydrocarbons</t>
   </si>
   <si>
@@ -243,16 +162,10 @@
     <t>avail_biomass</t>
   </si>
   <si>
-    <t>"Availability of local biomass"</t>
-  </si>
-  <si>
     <t>c_op_elec</t>
   </si>
   <si>
     <t>f_max_pv</t>
-  </si>
-  <si>
-    <t>"Maximum capacity of pv panels"</t>
   </si>
   <si>
     <t>delta_change_lt_heat</t>
@@ -321,24 +234,15 @@
     <t>f_max_nuclear_smr</t>
   </si>
   <si>
-    <t>"Potential availability of SMR nuclear, from 2040 at the earliest"</t>
-  </si>
-  <si>
     <t>passenger_eud</t>
   </si>
   <si>
-    <t>"End-use demand of households"</t>
-  </si>
-  <si>
     <t>households_eud</t>
   </si>
   <si>
     <t>industry_eud</t>
   </si>
   <si>
-    <t>"End-use demand of industry"</t>
-  </si>
-  <si>
     <t>services_eud</t>
   </si>
   <si>
@@ -363,9 +267,6 @@
     <t>Meaning_full</t>
   </si>
   <si>
-    <t>"Operational cost of imported fossil hydrocarbons"</t>
-  </si>
-  <si>
     <t>Interest rate</t>
   </si>
   <si>
@@ -402,21 +303,9 @@
     <t>Efficiency e-engine</t>
   </si>
   <si>
-    <t>Available biomass</t>
-  </si>
-  <si>
     <t>Max capacity PV</t>
   </si>
   <si>
-    <t>Share change freight transport</t>
-  </si>
-  <si>
-    <t>Share change pass. mobility</t>
-  </si>
-  <si>
-    <t>Share change LT-heat</t>
-  </si>
-  <si>
     <t>Max share of pub. transport</t>
   </si>
   <si>
@@ -435,27 +324,18 @@
     <t>Capex car</t>
   </si>
   <si>
-    <t>Variable opex</t>
-  </si>
-  <si>
     <t>Capex efficiency measures</t>
   </si>
   <si>
     <t>Capex ICE</t>
   </si>
   <si>
-    <t>Capex e-engine</t>
-  </si>
-  <si>
     <t>Purchase electricity</t>
   </si>
   <si>
     <t>Capex PV</t>
   </si>
   <si>
-    <t>Capex grid</t>
-  </si>
-  <si>
     <t>Capex bus</t>
   </si>
   <si>
@@ -466,6 +346,135 @@
   </si>
   <si>
     <t>Capex grid reinforcement</t>
+  </si>
+  <si>
+    <t>Operational cost of imported fossil hydrocarbons</t>
+  </si>
+  <si>
+    <t>Investment cost of FC propulsion system</t>
+  </si>
+  <si>
+    <t>Investment cost of cars</t>
+  </si>
+  <si>
+    <t>Variability in maintenance cost</t>
+  </si>
+  <si>
+    <t>Investment cost to increase efficiency of the system</t>
+  </si>
+  <si>
+    <t>Investment cost of IC propulsion system</t>
+  </si>
+  <si>
+    <t>Investment cost of e-propulsion system</t>
+  </si>
+  <si>
+    <t>Operational cost of imported electricity</t>
+  </si>
+  <si>
+    <t>Efficiency of FC propulsion system</t>
+  </si>
+  <si>
+    <t>End-use demand of households</t>
+  </si>
+  <si>
+    <t>Investment cost of PV</t>
+  </si>
+  <si>
+    <t>End-use demand of passenger mobility</t>
+  </si>
+  <si>
+    <t>Investment in the power grid'</t>
+  </si>
+  <si>
+    <t>End-use demand of space heating</t>
+  </si>
+  <si>
+    <t>Investment cost of buses</t>
+  </si>
+  <si>
+    <t>Maximum capacity of onshore wind</t>
+  </si>
+  <si>
+    <t>Available imported electricity</t>
+  </si>
+  <si>
+    <t>Load factor of PV</t>
+  </si>
+  <si>
+    <t>Operational cost of imported electrofuels</t>
+  </si>
+  <si>
+    <t>Load factor of wind turbines</t>
+  </si>
+  <si>
+    <t>Maximum capacity of offshore wind</t>
+  </si>
+  <si>
+    <t>Extra investment in the power grid due to VRES</t>
+  </si>
+  <si>
+    <t>Efficiency of e-propulsion system</t>
+  </si>
+  <si>
+    <t>Availability of local biomass</t>
+  </si>
+  <si>
+    <t>Maximum capacity of pv panels</t>
+  </si>
+  <si>
+    <t>Change of share of freight transport</t>
+  </si>
+  <si>
+    <t>Change of share of passenger transport</t>
+  </si>
+  <si>
+    <t>Change of share of low-temperature heat</t>
+  </si>
+  <si>
+    <t>Maximum share of pax-transport supplied by public transport</t>
+  </si>
+  <si>
+    <t>Potential availability of SMR nuclear, from 2040 at the earliest</t>
+  </si>
+  <si>
+    <t>End-use demand of industry</t>
+  </si>
+  <si>
+    <t>Variable opex of technologies</t>
+  </si>
+  <si>
+    <t>Capex power grid</t>
+  </si>
+  <si>
+    <t>Available local biomass</t>
+  </si>
+  <si>
+    <t>Modal share change pass. mobility</t>
+  </si>
+  <si>
+    <t>Modal share change LT-heat</t>
+  </si>
+  <si>
+    <t>Modal share change freight mobility</t>
+  </si>
+  <si>
+    <t>c_inv_nuclear_smr</t>
+  </si>
+  <si>
+    <t>Investment cost of nuclear small modular reactors</t>
+  </si>
+  <si>
+    <t>This range of this uncertainty has been taken from PATHS2050</t>
+  </si>
+  <si>
+    <t>Capex electric motor</t>
+  </si>
+  <si>
+    <t>Capex SMR</t>
+  </si>
+  <si>
+    <t>Operational cost of imported biofuels</t>
   </si>
 </sst>
 </file>
@@ -921,37 +930,37 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>82</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>95</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="B3" s="3"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>72</v>
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>73</v>
+        <v>44</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
-        <v>74</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>96</v>
+        <v>64</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
@@ -972,16 +981,17 @@
   <dimension ref="A1:G36"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="106" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="31.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="54.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18" customWidth="1"/>
+    <col min="5" max="5" width="42.5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="19" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -990,56 +1000,56 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>73</v>
       </c>
       <c r="C1" t="s">
-        <v>97</v>
+        <v>65</v>
       </c>
       <c r="D1" t="s">
-        <v>77</v>
+        <v>48</v>
       </c>
       <c r="E1" t="s">
-        <v>78</v>
+        <v>49</v>
       </c>
       <c r="F1" t="s">
-        <v>70</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="D2">
         <v>2</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="F2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B3" t="s">
-        <v>120</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
-        <v>14</v>
+        <v>94</v>
       </c>
       <c r="D3">
         <v>1</v>
       </c>
       <c r="E3" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F3" t="s">
         <v>7</v>
@@ -1047,22 +1057,22 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B4" t="s">
-        <v>121</v>
+        <v>84</v>
       </c>
       <c r="C4" t="s">
-        <v>16</v>
+        <v>95</v>
       </c>
       <c r="D4">
         <v>1</v>
       </c>
       <c r="E4" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -1070,16 +1080,16 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>96</v>
       </c>
       <c r="D5">
         <v>1</v>
       </c>
       <c r="E5" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F5" t="s">
         <v>3</v>
@@ -1087,22 +1097,22 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>123</v>
+        <v>85</v>
       </c>
       <c r="C6" t="s">
-        <v>19</v>
+        <v>97</v>
       </c>
       <c r="D6">
         <v>1</v>
       </c>
       <c r="E6" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F6" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -1110,16 +1120,16 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>99</v>
+        <v>66</v>
       </c>
       <c r="C7" t="s">
-        <v>21</v>
+        <v>66</v>
       </c>
       <c r="D7">
         <v>1</v>
       </c>
       <c r="E7" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F7" t="s">
         <v>1</v>
@@ -1127,39 +1137,39 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>86</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>98</v>
       </c>
       <c r="D8">
         <v>1</v>
       </c>
       <c r="E8" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F8" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>125</v>
+        <v>133</v>
       </c>
       <c r="C9" t="s">
-        <v>23</v>
+        <v>99</v>
       </c>
       <c r="D9">
         <v>1</v>
       </c>
       <c r="E9" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F9" t="s">
         <v>7</v>
@@ -1167,79 +1177,79 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B10" t="s">
-        <v>126</v>
+        <v>87</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>100</v>
       </c>
       <c r="D10">
         <v>2</v>
       </c>
       <c r="E10" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="F10" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>67</v>
       </c>
       <c r="C11" t="s">
-        <v>27</v>
+        <v>101</v>
       </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F11" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>101</v>
+        <v>68</v>
       </c>
       <c r="C12" t="s">
-        <v>86</v>
+        <v>102</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="F12" t="s">
-        <v>91</v>
+        <v>59</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B13" t="s">
-        <v>127</v>
+        <v>88</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>103</v>
       </c>
       <c r="D13">
         <v>1</v>
       </c>
       <c r="E13" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F13" t="s">
         <v>7</v>
@@ -1247,99 +1257,99 @@
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>102</v>
+        <v>69</v>
       </c>
       <c r="C14" t="s">
-        <v>31</v>
+        <v>104</v>
       </c>
       <c r="D14">
         <v>3</v>
       </c>
       <c r="E14" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="F14" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B15" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="C15" t="s">
-        <v>33</v>
+        <v>105</v>
       </c>
       <c r="D15">
         <v>1</v>
       </c>
       <c r="E15" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F15" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="B16" s="6" t="s">
-        <v>103</v>
+        <v>70</v>
       </c>
       <c r="C16" t="s">
-        <v>34</v>
+        <v>106</v>
       </c>
       <c r="D16">
         <v>3</v>
       </c>
       <c r="E16" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="F16" t="s">
-        <v>92</v>
+        <v>60</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B17" t="s">
-        <v>129</v>
+        <v>89</v>
       </c>
       <c r="C17" t="s">
-        <v>35</v>
+        <v>107</v>
       </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F17" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>71</v>
       </c>
       <c r="C18" t="s">
-        <v>36</v>
+        <v>108</v>
       </c>
       <c r="D18">
         <v>1</v>
       </c>
       <c r="E18" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F18" t="s">
         <v>2</v>
@@ -1347,39 +1357,39 @@
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B19" t="s">
-        <v>105</v>
+        <v>72</v>
       </c>
       <c r="C19" t="s">
-        <v>37</v>
+        <v>109</v>
       </c>
       <c r="D19">
         <v>1</v>
       </c>
       <c r="E19" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F19" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>74</v>
       </c>
       <c r="C20" t="s">
-        <v>39</v>
+        <v>110</v>
       </c>
       <c r="D20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E20" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F20" t="s">
         <v>8</v>
@@ -1390,19 +1400,19 @@
         <v>9</v>
       </c>
       <c r="B21" t="s">
-        <v>130</v>
+        <v>90</v>
       </c>
       <c r="C21" t="s">
-        <v>41</v>
+        <v>111</v>
       </c>
       <c r="D21">
         <v>2</v>
       </c>
       <c r="E21" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="F21" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1410,36 +1420,36 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
       <c r="C22" t="s">
-        <v>40</v>
+        <v>135</v>
       </c>
       <c r="D22">
         <v>2</v>
       </c>
       <c r="E22" t="s">
-        <v>81</v>
+        <v>52</v>
       </c>
       <c r="F22" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>75</v>
       </c>
       <c r="C23" t="s">
-        <v>42</v>
+        <v>112</v>
       </c>
       <c r="D23">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E23" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F23" t="s">
         <v>8</v>
@@ -1447,19 +1457,19 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B24" t="s">
-        <v>109</v>
+        <v>76</v>
       </c>
       <c r="C24" t="s">
-        <v>43</v>
+        <v>113</v>
       </c>
       <c r="D24">
         <v>1</v>
       </c>
       <c r="E24" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F24" t="s">
         <v>2</v>
@@ -1470,76 +1480,76 @@
         <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>132</v>
+        <v>92</v>
       </c>
       <c r="C25" t="s">
-        <v>44</v>
+        <v>114</v>
       </c>
       <c r="D25">
         <v>1</v>
       </c>
       <c r="E25" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F25" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B26" t="s">
-        <v>110</v>
+        <v>77</v>
       </c>
       <c r="C26" t="s">
-        <v>29</v>
+        <v>115</v>
       </c>
       <c r="D26">
         <v>1</v>
       </c>
       <c r="E26" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F26" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B27" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>116</v>
       </c>
       <c r="D27">
         <v>1</v>
       </c>
       <c r="E27" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F27" t="s">
-        <v>38</v>
+        <v>20</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B28" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
       <c r="C28" t="s">
-        <v>68</v>
+        <v>117</v>
       </c>
       <c r="D28">
         <v>1</v>
       </c>
       <c r="E28" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F28" t="s">
         <v>2</v>
@@ -1550,19 +1560,19 @@
         <v>12</v>
       </c>
       <c r="B29" t="s">
-        <v>113</v>
+        <v>129</v>
       </c>
       <c r="C29" t="s">
-        <v>45</v>
+        <v>118</v>
       </c>
       <c r="D29">
         <v>1</v>
       </c>
       <c r="E29" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F29" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1570,39 +1580,39 @@
         <v>13</v>
       </c>
       <c r="B30" t="s">
-        <v>114</v>
+        <v>127</v>
       </c>
       <c r="C30" t="s">
-        <v>46</v>
+        <v>119</v>
       </c>
       <c r="D30">
         <v>1</v>
       </c>
       <c r="E30" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F30" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>115</v>
+        <v>128</v>
       </c>
       <c r="C31" t="s">
-        <v>47</v>
+        <v>120</v>
       </c>
       <c r="D31">
         <v>1</v>
       </c>
       <c r="E31" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F31" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1610,78 +1620,125 @@
         <v>6</v>
       </c>
       <c r="B32" t="s">
-        <v>116</v>
+        <v>79</v>
       </c>
       <c r="C32" t="s">
-        <v>24</v>
+        <v>121</v>
       </c>
       <c r="D32">
         <v>1</v>
       </c>
       <c r="E32" t="s">
-        <v>79</v>
+        <v>50</v>
       </c>
       <c r="F32" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B33" t="s">
-        <v>117</v>
+        <v>80</v>
       </c>
       <c r="C33" t="s">
-        <v>84</v>
+        <v>122</v>
       </c>
       <c r="D33" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="E33" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="F33" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="G33" t="s">
-        <v>94</v>
+        <v>62</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B34" s="6" t="s">
-        <v>118</v>
+        <v>81</v>
       </c>
       <c r="C34" t="s">
-        <v>89</v>
+        <v>123</v>
       </c>
       <c r="D34">
         <v>3</v>
       </c>
       <c r="E34" t="s">
-        <v>80</v>
+        <v>51</v>
       </c>
       <c r="F34" t="s">
-        <v>93</v>
+        <v>61</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35" t="s">
+        <v>50</v>
+      </c>
+      <c r="F35" t="s">
+        <v>17</v>
+      </c>
+      <c r="G35" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
       <c r="C36" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="D2:D35">
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="F2:F35">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{208BE893-0ADC-A143-8FC7-0629E6D45632}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1697,15 +1754,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>-0.64264885308877462</v>
@@ -1716,7 +1773,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>-0.39600000000000002</v>
@@ -1728,7 +1785,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
         <v>-0.21599999999999997</v>
@@ -1750,7 +1807,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>-0.39300000000000002</v>
@@ -1772,7 +1829,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1">
         <v>-0.21599999999999997</v>
@@ -1783,7 +1840,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1">
         <v>-0.39600000000000002</v>
@@ -1794,7 +1851,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1">
         <v>-0.64264885308877462</v>
@@ -1805,7 +1862,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1">
         <v>-0.28700000000000003</v>
@@ -1816,7 +1873,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1">
         <v>-0.13779293938892206</v>
@@ -1827,7 +1884,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1">
         <v>-0.39600000000000002</v>
@@ -1838,7 +1895,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1">
         <v>-7.4661215202011591E-2</v>
@@ -1849,7 +1906,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1">
         <v>-0.39300000000000002</v>
@@ -1860,7 +1917,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1">
         <v>-0.14341697944019161</v>
@@ -1871,7 +1928,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1">
         <v>-0.21599999999999997</v>
@@ -1882,7 +1939,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>-0.24100000000000002</v>
@@ -1893,7 +1950,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1">
         <v>-0.3209999999999999</v>
@@ -1904,7 +1961,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1">
         <v>-0.22141466405484653</v>
@@ -1937,7 +1994,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1">
         <v>-0.22141466405484653</v>
@@ -1948,7 +2005,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1">
         <v>-0.24100000000000002</v>
@@ -1970,7 +2027,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1">
         <v>-0.28700000000000003</v>
@@ -1981,7 +2038,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1">
         <v>-0.3209999999999999</v>
@@ -1992,7 +2049,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1">
         <v>-0.24100000000000002</v>
@@ -2025,7 +2082,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1">
         <v>-0.3</v>
@@ -2047,7 +2104,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -2058,13 +2115,24 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1">
         <v>-0.20541415322547246</v>
       </c>
       <c r="C34" s="1">
         <v>0.15961025604371842</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.44</v>
       </c>
     </row>
   </sheetData>
@@ -2074,10 +2142,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B769D500-4815-264F-8946-7951AD07CA0A}">
-  <dimension ref="A1:G34"/>
+  <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A25"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2092,15 +2160,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>-0.64264885308877462</v>
@@ -2111,7 +2179,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>-0.39600000000000002</v>
@@ -2123,7 +2191,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
         <v>-0.21599999999999997</v>
@@ -2145,7 +2213,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>-0.39300000000000002</v>
@@ -2167,7 +2235,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1">
         <v>-0.21599999999999997</v>
@@ -2178,7 +2246,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1">
         <v>-0.39600000000000002</v>
@@ -2189,7 +2257,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1">
         <v>-0.64264885308877462</v>
@@ -2200,7 +2268,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1">
         <v>-0.28700000000000003</v>
@@ -2211,7 +2279,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1">
         <f>((READ_ME!$A$9-1)/5*1+1)*YEAR_2025!B12</f>
@@ -2224,7 +2292,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1">
         <v>-0.39600000000000002</v>
@@ -2235,7 +2303,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1">
         <f>((READ_ME!$A$9-1)/5*1+1)*YEAR_2025!B14</f>
@@ -2248,7 +2316,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1">
         <v>-0.39300000000000002</v>
@@ -2259,7 +2327,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1">
         <f>((READ_ME!$A$9-1)/5*1+1)*YEAR_2025!B16</f>
@@ -2272,7 +2340,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1">
         <v>-0.21599999999999997</v>
@@ -2283,7 +2351,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>-0.24100000000000002</v>
@@ -2294,7 +2362,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1">
         <v>-0.3209999999999999</v>
@@ -2305,7 +2373,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1">
         <v>-0.22141466405484653</v>
@@ -2338,7 +2406,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1">
         <v>-0.22141466405484653</v>
@@ -2349,7 +2417,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1">
         <v>-0.24100000000000002</v>
@@ -2371,7 +2439,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1">
         <v>-0.28700000000000003</v>
@@ -2382,7 +2450,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1">
         <v>-0.3209999999999999</v>
@@ -2393,7 +2461,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1">
         <v>-0.24100000000000002</v>
@@ -2426,7 +2494,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1">
         <v>-0.3</v>
@@ -2448,7 +2516,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -2459,7 +2527,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1">
         <f>((READ_ME!$A$9-1)/5*1+1)*YEAR_2025!B34</f>
@@ -2468,6 +2536,17 @@
       <c r="C34" s="1">
         <f>((READ_ME!$A$9-1)/5*1+1)*YEAR_2025!C34</f>
         <v>0.17557128164809027</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.44</v>
       </c>
     </row>
   </sheetData>
@@ -2477,10 +2556,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E4663EE-44ED-084C-95B1-2CAE43A7A62D}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18:A26"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2494,15 +2573,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>-0.64264885308877462</v>
@@ -2513,7 +2592,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>-0.39600000000000002</v>
@@ -2524,7 +2603,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
         <v>-0.21599999999999997</v>
@@ -2546,7 +2625,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>-0.39300000000000002</v>
@@ -2568,7 +2647,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1">
         <v>-0.21599999999999997</v>
@@ -2579,7 +2658,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1">
         <v>-0.39600000000000002</v>
@@ -2590,7 +2669,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1">
         <v>-0.64264885308877462</v>
@@ -2601,7 +2680,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1">
         <v>-0.28700000000000003</v>
@@ -2612,7 +2691,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1">
         <f>((READ_ME!$A$9-1)/5*2+1)*YEAR_2025!B12</f>
@@ -2625,7 +2704,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1">
         <v>-0.39600000000000002</v>
@@ -2636,7 +2715,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1">
         <f>((READ_ME!$A$9-1)/5*2+1)*YEAR_2025!B14</f>
@@ -2649,7 +2728,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1">
         <v>-0.39300000000000002</v>
@@ -2660,7 +2739,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1">
         <f>((READ_ME!$A$9-1)/5*2+1)*YEAR_2025!B16</f>
@@ -2673,7 +2752,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1">
         <v>-0.21599999999999997</v>
@@ -2684,7 +2763,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>-0.24100000000000002</v>
@@ -2695,7 +2774,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1">
         <v>-0.3209999999999999</v>
@@ -2706,7 +2785,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1">
         <v>-0.22141466405484653</v>
@@ -2739,7 +2818,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1">
         <v>-0.22141466405484653</v>
@@ -2750,7 +2829,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1">
         <v>-0.24100000000000002</v>
@@ -2772,7 +2851,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1">
         <v>-0.28700000000000003</v>
@@ -2783,7 +2862,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1">
         <v>-0.3209999999999999</v>
@@ -2794,7 +2873,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1">
         <v>-0.24100000000000002</v>
@@ -2827,7 +2906,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1">
         <v>-0.3</v>
@@ -2849,7 +2928,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -2860,7 +2939,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1">
         <f>((READ_ME!$A$9-1)/5*2+1)*YEAR_2025!B34</f>
@@ -2869,6 +2948,17 @@
       <c r="C34" s="1">
         <f>((READ_ME!$A$9-1)/5*2+1)*YEAR_2025!C34</f>
         <v>0.19153230725246209</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.44</v>
       </c>
     </row>
   </sheetData>
@@ -2878,10 +2968,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE79AA38-4E52-0649-9324-59F4BFECC736}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:A23"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2895,15 +2985,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>-0.64264885308877462</v>
@@ -2914,7 +3004,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>-0.39600000000000002</v>
@@ -2925,7 +3015,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
         <v>-0.21599999999999997</v>
@@ -2947,7 +3037,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>-0.39300000000000002</v>
@@ -2969,7 +3059,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1">
         <v>-0.21599999999999997</v>
@@ -2980,7 +3070,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1">
         <v>-0.39600000000000002</v>
@@ -2991,7 +3081,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1">
         <v>-0.64264885308877462</v>
@@ -3002,7 +3092,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1">
         <v>-0.28700000000000003</v>
@@ -3013,7 +3103,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1">
         <f>((READ_ME!$A$9-1)/5*3+1)*YEAR_2025!B12</f>
@@ -3026,7 +3116,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1">
         <v>-0.39600000000000002</v>
@@ -3037,7 +3127,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1">
         <f>((READ_ME!$A$9-1)/5*3+1)*YEAR_2025!B14</f>
@@ -3050,7 +3140,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1">
         <v>-0.39300000000000002</v>
@@ -3061,7 +3151,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1">
         <f>((READ_ME!$A$9-1)/5*3+1)*YEAR_2025!B16</f>
@@ -3074,7 +3164,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1">
         <v>-0.21599999999999997</v>
@@ -3085,7 +3175,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>-0.24100000000000002</v>
@@ -3096,7 +3186,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1">
         <v>-0.3209999999999999</v>
@@ -3107,7 +3197,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1">
         <v>-0.22141466405484653</v>
@@ -3140,7 +3230,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1">
         <v>-0.22141466405484653</v>
@@ -3151,7 +3241,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1">
         <v>-0.24100000000000002</v>
@@ -3173,7 +3263,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1">
         <v>-0.28700000000000003</v>
@@ -3184,7 +3274,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1">
         <v>-0.3209999999999999</v>
@@ -3195,7 +3285,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1">
         <v>-0.24100000000000002</v>
@@ -3228,7 +3318,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1">
         <v>-0.3</v>
@@ -3250,7 +3340,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B33" s="5">
         <v>0</v>
@@ -3261,7 +3351,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1">
         <f>((READ_ME!$A$9-1)/5*3+1)*YEAR_2025!B34</f>
@@ -3270,6 +3360,17 @@
       <c r="C34" s="1">
         <f>((READ_ME!$A$9-1)/5*3+1)*YEAR_2025!C34</f>
         <v>0.20749333285683397</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.44</v>
       </c>
     </row>
   </sheetData>
@@ -3279,10 +3380,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB9CEDAD-A2BB-9A46-9C45-7E4D665515C6}">
-  <dimension ref="A1:C34"/>
+  <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3296,15 +3397,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>-0.64264885308877462</v>
@@ -3315,7 +3416,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>-0.39600000000000002</v>
@@ -3326,7 +3427,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
         <v>-0.21599999999999997</v>
@@ -3348,7 +3449,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>-0.39300000000000002</v>
@@ -3370,7 +3471,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1">
         <v>-0.21599999999999997</v>
@@ -3381,7 +3482,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1">
         <v>-0.39600000000000002</v>
@@ -3392,7 +3493,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1">
         <v>-0.64264885308877462</v>
@@ -3403,7 +3504,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1">
         <v>-0.28700000000000003</v>
@@ -3414,7 +3515,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1">
         <f>((READ_ME!$A$9-1)/5*4+1)*YEAR_2025!B12</f>
@@ -3427,7 +3528,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1">
         <v>-0.39600000000000002</v>
@@ -3438,7 +3539,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1">
         <f>((READ_ME!$A$9-1)/5*4+1)*YEAR_2025!B14</f>
@@ -3451,7 +3552,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1">
         <v>-0.39300000000000002</v>
@@ -3462,7 +3563,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1">
         <f>((READ_ME!$A$9-1)/5*4+1)*YEAR_2025!B16</f>
@@ -3475,7 +3576,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1">
         <v>-0.21599999999999997</v>
@@ -3486,7 +3587,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>-0.24100000000000002</v>
@@ -3497,7 +3598,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1">
         <v>-0.3209999999999999</v>
@@ -3508,7 +3609,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1">
         <v>-0.22141466405484653</v>
@@ -3541,7 +3642,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1">
         <v>-0.22141466405484653</v>
@@ -3552,7 +3653,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1">
         <v>-0.24100000000000002</v>
@@ -3574,7 +3675,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1">
         <v>-0.28700000000000003</v>
@@ -3585,7 +3686,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1">
         <v>-0.3209999999999999</v>
@@ -3596,7 +3697,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1">
         <v>-0.24100000000000002</v>
@@ -3629,7 +3730,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1">
         <v>-0.3</v>
@@ -3651,7 +3752,7 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B33" s="5">
         <v>0</v>
@@ -3662,7 +3763,7 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1">
         <f>((READ_ME!$A$9-1)/5*4+1)*YEAR_2025!B34</f>
@@ -3671,6 +3772,17 @@
       <c r="C34" s="1">
         <f>((READ_ME!$A$9-1)/5*4+1)*YEAR_2025!C34</f>
         <v>0.22345435846120579</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.44</v>
       </c>
     </row>
   </sheetData>
@@ -3683,7 +3795,7 @@
   <dimension ref="A1:G35"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F29" sqref="F29"/>
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3697,15 +3809,15 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>75</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>76</v>
+        <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>48</v>
+        <v>21</v>
       </c>
       <c r="B2" s="1">
         <v>-0.64264885308877462</v>
@@ -3716,7 +3828,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>50</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1">
         <v>-0.39600000000000002</v>
@@ -3727,7 +3839,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>49</v>
+        <v>22</v>
       </c>
       <c r="B4" s="1">
         <v>-0.21599999999999997</v>
@@ -3749,7 +3861,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>51</v>
+        <v>24</v>
       </c>
       <c r="B6" s="1">
         <v>-0.39300000000000002</v>
@@ -3771,7 +3883,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>25</v>
       </c>
       <c r="B8" s="1">
         <v>-0.21599999999999997</v>
@@ -3782,7 +3894,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>26</v>
       </c>
       <c r="B9" s="1">
         <v>-0.39600000000000002</v>
@@ -3793,7 +3905,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>66</v>
+        <v>38</v>
       </c>
       <c r="B10" s="1">
         <v>-0.64264885308877462</v>
@@ -3804,7 +3916,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B11" s="1">
         <v>-0.28700000000000003</v>
@@ -3815,7 +3927,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="6" t="s">
-        <v>87</v>
+        <v>56</v>
       </c>
       <c r="B12" s="1">
         <f>((READ_ME!$A$9-1)/5*5+1)*YEAR_2025!B12</f>
@@ -3828,7 +3940,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="B13" s="1">
         <v>-0.39600000000000002</v>
@@ -3839,7 +3951,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="6" t="s">
-        <v>85</v>
+        <v>55</v>
       </c>
       <c r="B14" s="1">
         <f>((READ_ME!$A$9-1)/5*5+1)*YEAR_2025!B14</f>
@@ -3852,7 +3964,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>56</v>
+        <v>29</v>
       </c>
       <c r="B15" s="1">
         <v>-0.39300000000000002</v>
@@ -3863,7 +3975,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="6" t="s">
-        <v>90</v>
+        <v>58</v>
       </c>
       <c r="B16" s="1">
         <f>((READ_ME!$A$9-1)/5*5+1)*YEAR_2025!B16</f>
@@ -3876,7 +3988,7 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>30</v>
       </c>
       <c r="B17" s="1">
         <v>-0.21599999999999997</v>
@@ -3887,7 +3999,7 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>58</v>
+        <v>31</v>
       </c>
       <c r="B18" s="1">
         <v>-0.24100000000000002</v>
@@ -3898,7 +4010,7 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>59</v>
+        <v>32</v>
       </c>
       <c r="B19" s="1">
         <v>-0.3209999999999999</v>
@@ -3909,7 +4021,7 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="6" t="s">
-        <v>60</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1">
         <v>-0.22141466405484653</v>
@@ -3942,7 +4054,7 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="6" t="s">
-        <v>61</v>
+        <v>34</v>
       </c>
       <c r="B23" s="1">
         <v>-0.22141466405484653</v>
@@ -3953,7 +4065,7 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
-        <v>62</v>
+        <v>35</v>
       </c>
       <c r="B24" s="1">
         <v>-0.24100000000000002</v>
@@ -3975,7 +4087,7 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>63</v>
+        <v>36</v>
       </c>
       <c r="B26" s="1">
         <v>-0.28700000000000003</v>
@@ -3986,7 +4098,7 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>64</v>
+        <v>37</v>
       </c>
       <c r="B27" s="1">
         <v>-0.3209999999999999</v>
@@ -3997,7 +4109,7 @@
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>67</v>
+        <v>39</v>
       </c>
       <c r="B28" s="1">
         <v>-0.24100000000000002</v>
@@ -4030,7 +4142,7 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
-        <v>69</v>
+        <v>40</v>
       </c>
       <c r="B31" s="1">
         <v>-0.3</v>
@@ -4052,7 +4164,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
-        <v>83</v>
+        <v>54</v>
       </c>
       <c r="B33" s="5">
         <v>0</v>
@@ -4063,7 +4175,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A34" s="6" t="s">
-        <v>88</v>
+        <v>57</v>
       </c>
       <c r="B34" s="1">
         <f>((READ_ME!$A$9-1)/5*5+1)*YEAR_2025!B34</f>
@@ -4075,6 +4187,15 @@
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>130</v>
+      </c>
+      <c r="B35" s="1">
+        <v>-0.4</v>
+      </c>
+      <c r="C35" s="1">
+        <v>0.44</v>
+      </c>
       <c r="F35" s="1"/>
       <c r="G35" s="1"/>
     </row>

</xml_diff>